<commit_message>
chinh sua ket noi va covert data
</commit_message>
<xml_diff>
--- a/WindowsFormsApp1/Files/data_dongco_1.xlsx
+++ b/WindowsFormsApp1/Files/data_dongco_1.xlsx
@@ -9,17 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="564">
   <si>
     <t>Máy1_SPD Tuabin tăng áp 1</t>
   </si>
@@ -1705,6 +1708,12 @@
   </si>
   <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -2689,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>241</v>
+        <v>562</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2770,7 +2779,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>241</v>
+        <v>563</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -7328,6 +7337,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
them code lay data tu plc
</commit_message>
<xml_diff>
--- a/WindowsFormsApp1/Files/data_dongco_1.xlsx
+++ b/WindowsFormsApp1/Files/data_dongco_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20490" windowHeight="8235"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="562">
   <si>
     <t>Máy1_SPD Tuabin tăng áp 1</t>
   </si>
@@ -1708,12 +1708,6 @@
   </si>
   <si>
     <t>200</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.6</t>
   </si>
 </sst>
 </file>
@@ -2699,7 +2693,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2743,8 +2737,8 @@
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>45</v>
+      <c r="C2" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>49</v>
@@ -2756,7 +2750,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>562</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2767,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>49</v>
@@ -2779,7 +2773,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>563</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3203,8 +3197,8 @@
       <c r="B22" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>45</v>
+      <c r="C22" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>49</v>
@@ -3227,7 +3221,7 @@
         <v>51</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D23" s="13" t="s">
         <v>49</v>
@@ -3663,8 +3657,8 @@
       <c r="B42" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>45</v>
+      <c r="C42" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>49</v>
@@ -3687,7 +3681,7 @@
         <v>71</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" s="13" t="s">
         <v>49</v>
@@ -4123,8 +4117,8 @@
       <c r="B62" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="C62" s="7" t="s">
-        <v>45</v>
+      <c r="C62" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>49</v>
@@ -4147,7 +4141,7 @@
         <v>91</v>
       </c>
       <c r="C63" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>49</v>
@@ -4583,8 +4577,8 @@
       <c r="B82" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C82" s="7" t="s">
-        <v>45</v>
+      <c r="C82" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>49</v>
@@ -4607,7 +4601,7 @@
         <v>111</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D83" s="13" t="s">
         <v>49</v>
@@ -5043,8 +5037,8 @@
       <c r="B102" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C102" s="7" t="s">
-        <v>45</v>
+      <c r="C102" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D102" s="8" t="s">
         <v>49</v>
@@ -5067,7 +5061,7 @@
         <v>131</v>
       </c>
       <c r="C103" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D103" s="13" t="s">
         <v>49</v>
@@ -5503,8 +5497,8 @@
       <c r="B122" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="C122" s="7" t="s">
-        <v>45</v>
+      <c r="C122" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>49</v>
@@ -5527,7 +5521,7 @@
         <v>151</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D123" s="13" t="s">
         <v>49</v>
@@ -5963,8 +5957,8 @@
       <c r="B142" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="C142" s="7" t="s">
-        <v>45</v>
+      <c r="C142" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>49</v>
@@ -5987,7 +5981,7 @@
         <v>171</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D143" s="13" t="s">
         <v>49</v>
@@ -6423,8 +6417,8 @@
       <c r="B162" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="C162" s="7" t="s">
-        <v>45</v>
+      <c r="C162" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D162" s="8" t="s">
         <v>49</v>
@@ -6447,7 +6441,7 @@
         <v>191</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D163" s="13" t="s">
         <v>49</v>
@@ -6883,8 +6877,8 @@
       <c r="B182" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C182" s="7" t="s">
-        <v>45</v>
+      <c r="C182" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D182" s="8" t="s">
         <v>49</v>
@@ -6907,7 +6901,7 @@
         <v>211</v>
       </c>
       <c r="C183" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D183" s="13" t="s">
         <v>49</v>

</xml_diff>